<commit_message>
Dataset minor correction - removing unexpected birthdate and first manually created example
</commit_message>
<xml_diff>
--- a/UC-Serafe/EWR-Dataset-fiction/EWR_ResidencesPrincipales.xlsx
+++ b/UC-Serafe/EWR-Dataset-fiction/EWR_ResidencesPrincipales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hessoit-my.sharepoint.com/personal/fabian_cretton_hes-so_ch/Documents/Fabian/BK 2024/UC Serafe/EWR-Dataset-fiction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DB114E441178AC67DF4D46695F050693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C425AFD-CFA5-4DEC-8BAD-FD0EBD03AA50}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="11_AD4DB114E441178AC67DF4D46695F050693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D93465B-3012-4E0E-B46B-3ED117BADC96}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Boulevard des Alpes</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>endDate</t>
-  </si>
-  <si>
-    <t>birthDate</t>
   </si>
 </sst>
 </file>
@@ -477,22 +474,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="7" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -517,11 +512,8 @@
       <c r="H1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1234567890</v>
       </c>
@@ -546,11 +538,8 @@
       <c r="H2" s="4">
         <v>19652</v>
       </c>
-      <c r="I2" s="5">
-        <v>4679</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2345678901</v>
       </c>
@@ -575,11 +564,8 @@
       <c r="H3" s="4">
         <v>39982</v>
       </c>
-      <c r="I3" s="5">
-        <v>13592</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3456789012</v>
       </c>
@@ -604,11 +590,8 @@
       <c r="H4" s="4">
         <v>21887</v>
       </c>
-      <c r="I4" s="5">
-        <v>14585</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4567890123</v>
       </c>
@@ -633,11 +616,8 @@
       <c r="H5" s="4">
         <v>39781</v>
       </c>
-      <c r="I5" s="5">
-        <v>16769</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5678901234</v>
       </c>
@@ -662,11 +642,8 @@
       <c r="H6" s="4">
         <v>38849</v>
       </c>
-      <c r="I6" s="5">
-        <v>17408</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6789012345</v>
       </c>
@@ -691,11 +668,8 @@
       <c r="H7" s="4">
         <v>40224</v>
       </c>
-      <c r="I7" s="5">
-        <v>18246</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7890123456</v>
       </c>
@@ -720,11 +694,8 @@
       <c r="H8" s="4">
         <v>38237</v>
       </c>
-      <c r="I8" s="5">
-        <v>18755</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8901234567</v>
       </c>
@@ -749,11 +720,8 @@
       <c r="H9" s="4">
         <v>40506</v>
       </c>
-      <c r="I9" s="5">
-        <v>26429</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9012345678</v>
       </c>
@@ -778,11 +746,8 @@
       <c r="H10" s="4">
         <v>40055</v>
       </c>
-      <c r="I10" s="5">
-        <v>27872</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>123456789</v>
       </c>
@@ -807,11 +772,8 @@
       <c r="H11" s="4">
         <v>38461</v>
       </c>
-      <c r="I11" s="5">
-        <v>28145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9876543210</v>
       </c>
@@ -836,11 +798,8 @@
       <c r="H12" s="4">
         <v>40461</v>
       </c>
-      <c r="I12" s="5">
-        <v>33340</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8765432109</v>
       </c>
@@ -865,11 +824,8 @@
       <c r="H13" s="4">
         <v>40264</v>
       </c>
-      <c r="I13" s="5">
-        <v>33449</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7654321098</v>
       </c>
@@ -894,11 +850,8 @@
       <c r="H14" s="4">
         <v>39265</v>
       </c>
-      <c r="I14" s="5">
-        <v>35136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6543210987</v>
       </c>
@@ -923,11 +876,8 @@
       <c r="H15" s="4">
         <v>42322</v>
       </c>
-      <c r="I15" s="5">
-        <v>35816</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>5432109876</v>
       </c>
@@ -952,11 +902,8 @@
       <c r="H16" s="4">
         <v>40429</v>
       </c>
-      <c r="I16" s="5">
-        <v>36371</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4321098765</v>
       </c>
@@ -981,11 +928,8 @@
       <c r="H17" s="4">
         <v>43855</v>
       </c>
-      <c r="I17" s="5">
-        <v>38860</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3210987654</v>
       </c>
@@ -1010,11 +954,8 @@
       <c r="H18" s="4">
         <v>43585</v>
       </c>
-      <c r="I18" s="5">
-        <v>39926</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2109876543</v>
       </c>
@@ -1039,11 +980,8 @@
       <c r="H19" s="5">
         <v>43372</v>
       </c>
-      <c r="I19" s="5">
-        <v>42642</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1098765432</v>
       </c>
@@ -1068,11 +1006,8 @@
       <c r="H20" s="5">
         <v>43752</v>
       </c>
-      <c r="I20" s="5">
-        <v>42657</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>987654321</v>
       </c>
@@ -1097,11 +1032,8 @@
       <c r="H21" s="5">
         <v>43740</v>
       </c>
-      <c r="I21" s="5">
-        <v>43648</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>9876543211</v>
       </c>
@@ -1126,11 +1058,8 @@
       <c r="H22" s="5">
         <v>15498</v>
       </c>
-      <c r="I22" s="5">
-        <v>8193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>8765432108</v>
       </c>
@@ -1155,11 +1084,8 @@
       <c r="H23" s="4">
         <v>40404</v>
       </c>
-      <c r="I23" s="5">
-        <v>28674</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>7654321095</v>
       </c>
@@ -1184,11 +1110,8 @@
       <c r="H24" s="4">
         <v>37321</v>
       </c>
-      <c r="I24" s="5">
-        <v>35430</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>6543210984</v>
       </c>
@@ -1213,11 +1136,8 @@
       <c r="H25" s="5">
         <v>41364</v>
       </c>
-      <c r="I25" s="5">
-        <v>40268</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>

</xml_diff>